<commit_message>
Cleaned up repo and updated readme
</commit_message>
<xml_diff>
--- a/doc/datasets.xlsx
+++ b/doc/datasets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13658"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13658" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart3" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>(ω + 1) conflicts</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
+    <t>literals</t>
   </si>
 </sst>
 </file>
@@ -4454,7 +4460,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="190" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
@@ -4882,10 +4888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4898,7 +4904,7 @@
     <col min="13" max="13" width="13.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="E1" s="5" t="s">
         <v>28</v>
       </c>
@@ -4911,7 +4917,7 @@
       </c>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4951,8 +4957,14 @@
       <c r="M2" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4992,8 +5004,18 @@
       <c r="M3">
         <v>7418</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N3">
+        <f>L3/J3</f>
+        <v>5411.5555555555557</v>
+      </c>
+      <c r="O3">
+        <v>2286</v>
+      </c>
+      <c r="P3" s="2">
+        <v>60199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5033,8 +5055,18 @@
       <c r="M4">
         <v>130043</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N4">
+        <f t="shared" ref="N4:N12" si="0">L4/J4</f>
+        <v>4507.3121019108285</v>
+      </c>
+      <c r="O4">
+        <v>7193</v>
+      </c>
+      <c r="P4">
+        <v>531836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5074,8 +5106,18 @@
       <c r="M5">
         <v>7552</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>19164.444444444445</v>
+      </c>
+      <c r="O5">
+        <v>1559</v>
+      </c>
+      <c r="P5">
+        <v>26819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5115,8 +5157,18 @@
       <c r="M6">
         <v>2521</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>14186.666666666666</v>
+      </c>
+      <c r="O6">
+        <v>1041</v>
+      </c>
+      <c r="P6">
+        <v>12909</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5156,8 +5208,18 @@
       <c r="M7">
         <v>2908</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>3680</v>
+      </c>
+      <c r="O7">
+        <v>1154</v>
+      </c>
+      <c r="P7">
+        <v>16091</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5197,8 +5259,18 @@
       <c r="M8">
         <v>352</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8">
+        <v>424</v>
+      </c>
+      <c r="P8">
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5238,8 +5310,18 @@
       <c r="M9">
         <v>49105</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>2859.4680867875036</v>
+      </c>
+      <c r="O9">
+        <v>5457</v>
+      </c>
+      <c r="P9">
+        <v>312068</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5280,8 +5362,18 @@
       <c r="M10">
         <v>1449426</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>6293.0731707317073</v>
+      </c>
+      <c r="O10">
+        <v>5220</v>
+      </c>
+      <c r="P10">
+        <v>265496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5321,8 +5413,18 @@
       <c r="M11">
         <v>22204</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>2209.6842105263158</v>
+      </c>
+      <c r="O11">
+        <v>3644</v>
+      </c>
+      <c r="P11">
+        <v>149737</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5362,8 +5464,18 @@
       <c r="M12">
         <v>440</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>1984</v>
+      </c>
+      <c r="O12">
+        <v>355</v>
+      </c>
+      <c r="P12">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -5399,7 +5511,7 @@
       </c>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -5434,7 +5546,7 @@
         <v>39.015599999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -5469,7 +5581,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>